<commit_message>
Corrected calculation for billing and collection
</commit_message>
<xml_diff>
--- a/dashboard/KAM_Dashboard_FY26.xlsx
+++ b/dashboard/KAM_Dashboard_FY26.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://crmnext-my.sharepoint.com/personal/devansh_goel_businessnext_com/Documents/Desktop/New folder/Code/kam-dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://crmnext-my.sharepoint.com/personal/devansh_goel_businessnext_com/Documents/Desktop/New folder/Code/dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_287AFBE6CB9CEE75FF8927CC49F99982C9141A9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87ACF9FC-5E06-4780-99C2-94D2E012895F}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="14_{9329AC9F-7251-4B51-8136-87E98A47E201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CAA2465-8F0A-48BB-B556-0CB1FB7AA628}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual KPIs" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,25 @@
     <sheet name="Weightages" sheetId="8" r:id="rId8"/>
     <sheet name="Instructions" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="105">
   <si>
     <t>KAM Dashboard - Annual KPIs</t>
   </si>
@@ -383,8 +396,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,13 +746,13 @@
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -833,26 +846,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -863,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -874,137 +890,147 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1">
+        <v>12.2401196</v>
+      </c>
+      <c r="C4" s="1">
         <v>4.1383649999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="1">
+        <v>45.873390749999999</v>
+      </c>
+      <c r="C5" s="1">
         <v>15.240641700000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>17.959842599999998</v>
+      </c>
+      <c r="C6" s="1">
         <v>13.327025299999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="1">
+        <v>35.709941299999997</v>
+      </c>
+      <c r="C7" s="1">
         <v>20.950151599999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="1">
+        <v>11.6152499</v>
+      </c>
+      <c r="C8" s="1">
         <v>5.5789846749999992</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="1">
+        <v>31.928199900000003</v>
+      </c>
+      <c r="C9" s="1">
         <v>21.451520899999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="1">
+        <v>31.396266600000004</v>
+      </c>
+      <c r="C10" s="1">
         <v>9.4403080999999993</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="1">
+        <v>39.890963999999997</v>
+      </c>
+      <c r="C11" s="1">
         <v>66.977550100000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="1">
+        <v>37.852322048000005</v>
+      </c>
+      <c r="C12" s="1">
         <v>26.671124347999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="1">
+        <v>31.732866250000001</v>
+      </c>
+      <c r="C13" s="1">
         <v>19.512248599999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="1">
+        <v>29.524683900000003</v>
+      </c>
+      <c r="C14" s="1">
         <v>7.6861787000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
+      <c r="B15" s="1">
+        <v>36.433806050000001</v>
+      </c>
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1012,7 +1038,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C3 A15:C15 A4:B14" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C3 A15 A4:A14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1022,19 +1048,19 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1064,10 +1090,10 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>10.587243711999999</v>
+      </c>
+      <c r="C4" s="1">
         <v>10.172505237999999</v>
       </c>
     </row>
@@ -1075,10 +1101,10 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>14.570945153199997</v>
+      </c>
+      <c r="C5" s="1">
         <v>16.232625200000001</v>
       </c>
     </row>
@@ -1086,10 +1112,10 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>13.042712700000001</v>
+      </c>
+      <c r="C6" s="1">
         <v>12.341751695000001</v>
       </c>
     </row>
@@ -1097,10 +1123,10 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>10.565674063500001</v>
+      </c>
+      <c r="C7" s="1">
         <v>14.565941799999999</v>
       </c>
     </row>
@@ -1108,10 +1134,10 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
-        <v>30</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>22.186550787999998</v>
+      </c>
+      <c r="C8" s="1">
         <v>10.404058984000001</v>
       </c>
     </row>
@@ -1119,10 +1145,10 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
-        <v>30</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1">
+        <v>27.562345714999999</v>
+      </c>
+      <c r="C9" s="1">
         <v>23.378130599999999</v>
       </c>
     </row>
@@ -1130,10 +1156,10 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1">
+        <v>21.088647905779997</v>
+      </c>
+      <c r="C10" s="1">
         <v>14.196419000000001</v>
       </c>
     </row>
@@ -1141,10 +1167,10 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>30</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="1">
+        <v>18.630064737999998</v>
+      </c>
+      <c r="C11" s="1">
         <v>13.919755455799999</v>
       </c>
     </row>
@@ -1152,10 +1178,10 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
-        <v>30</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1">
+        <v>20.465125691120001</v>
+      </c>
+      <c r="C12" s="1">
         <v>23.662476788000003</v>
       </c>
     </row>
@@ -1163,10 +1189,10 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>30</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1">
+        <v>14.031910436199999</v>
+      </c>
+      <c r="C13" s="1">
         <v>13.130050776999999</v>
       </c>
     </row>
@@ -1174,10 +1200,10 @@
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>30</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1">
+        <v>17.351059494974404</v>
+      </c>
+      <c r="C14" s="1">
         <v>9.3312188690000006</v>
       </c>
     </row>
@@ -1185,12 +1211,10 @@
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
+      <c r="B15" s="1">
+        <v>22.271835690400003</v>
+      </c>
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1198,29 +1222,29 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C3 A15:C15 A4:B14" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C3 A15 A4:A14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1250,45 +1274,77 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4">
-        <v>25</v>
-      </c>
-      <c r="C4">
-        <v>22</v>
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>21</v>
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
         <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7">
-        <v>25</v>
-      </c>
-      <c r="C7">
-        <v>15</v>
-      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1296,7 +1352,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C7" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C3 A4:A7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1312,13 +1368,13 @@
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1404,25 +1460,25 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1464,16 +1520,16 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3.1119899999999999E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>27.27</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>30.227573322000005</v>
       </c>
     </row>
@@ -1481,16 +1537,16 @@
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>13.95</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>19.833181799999998</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>27.27</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>32.60451681</v>
       </c>
     </row>
@@ -1498,16 +1554,16 @@
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>11.625</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>-0.70756160000000001</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>27.27</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>28.724957527000011</v>
       </c>
     </row>
@@ -1515,16 +1571,16 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>11.625</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>27.27</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>25.169769212999988</v>
       </c>
     </row>
@@ -1550,16 +1606,16 @@
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1746,20 +1802,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ADd label to graph
</commit_message>
<xml_diff>
--- a/dashboard/KAM_Dashboard_FY26.xlsx
+++ b/dashboard/KAM_Dashboard_FY26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://crmnext-my.sharepoint.com/personal/devansh_goel_businessnext_com/Documents/Desktop/New folder/Code/dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="14_{9329AC9F-7251-4B51-8136-87E98A47E201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CAA2465-8F0A-48BB-B556-0CB1FB7AA628}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="14_{9329AC9F-7251-4B51-8136-87E98A47E201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E0CF3F3-8A06-47F7-8312-ED56E94734FE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual KPIs" sheetId="1" r:id="rId1"/>
@@ -740,7 +740,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1460,7 +1460,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1599,11 +1599,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.4140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
Account Owner Drill Down
</commit_message>
<xml_diff>
--- a/dashboard/KAM_Dashboard_FY26.xlsx
+++ b/dashboard/KAM_Dashboard_FY26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://crmnext-my.sharepoint.com/personal/devansh_goel_businessnext_com/Documents/Desktop/New folder/Code/dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="14_{9329AC9F-7251-4B51-8136-87E98A47E201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E0CF3F3-8A06-47F7-8312-ED56E94734FE}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="14_{9329AC9F-7251-4B51-8136-87E98A47E201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09320084-D02C-40EE-A7C1-5E81A302B2E6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual KPIs" sheetId="1" r:id="rId1"/>
@@ -394,10 +394,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,7 +850,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -898,9 +899,9 @@
         <v>12.2401196</v>
       </c>
       <c r="C4" s="1">
-        <v>4.1383649999999994</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>4.233365</v>
+      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -911,9 +912,9 @@
         <v>45.873390749999999</v>
       </c>
       <c r="C5" s="1">
-        <v>15.240641700000001</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>14.377390500000001</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -923,9 +924,9 @@
         <v>17.959842599999998</v>
       </c>
       <c r="C6" s="1">
-        <v>13.327025299999999</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>13.1970253</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -935,9 +936,9 @@
         <v>35.709941299999997</v>
       </c>
       <c r="C7" s="1">
-        <v>20.950151599999998</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>20.910151599999999</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -947,9 +948,9 @@
         <v>11.6152499</v>
       </c>
       <c r="C8" s="1">
-        <v>5.5789846749999992</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>5.5789847000000004</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -959,9 +960,9 @@
         <v>31.928199900000003</v>
       </c>
       <c r="C9" s="1">
-        <v>21.451520899999998</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>21.392120899999998</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -971,9 +972,9 @@
         <v>31.396266600000004</v>
       </c>
       <c r="C10" s="1">
-        <v>9.4403080999999993</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>8.1453403000000009</v>
+      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -983,9 +984,9 @@
         <v>39.890963999999997</v>
       </c>
       <c r="C11" s="1">
-        <v>66.977550100000002</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>67.188736399999996</v>
+      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -995,9 +996,9 @@
         <v>37.852322048000005</v>
       </c>
       <c r="C12" s="1">
-        <v>26.671124347999999</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>24.515263399999998</v>
+      </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1007,9 +1008,9 @@
         <v>31.732866250000001</v>
       </c>
       <c r="C13" s="1">
-        <v>19.512248599999999</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>14.112248599999999</v>
+      </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1019,9 +1020,9 @@
         <v>29.524683900000003</v>
       </c>
       <c r="C14" s="1">
-        <v>7.6861787000000001</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>6.4880142999999997</v>
+      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1047,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1094,7 +1095,7 @@
         <v>10.587243711999999</v>
       </c>
       <c r="C4" s="1">
-        <v>10.172505237999999</v>
+        <v>10.1832961</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1105,7 +1106,7 @@
         <v>14.570945153199997</v>
       </c>
       <c r="C5" s="1">
-        <v>16.232625200000001</v>
+        <v>15.8174274</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1116,7 +1117,7 @@
         <v>13.042712700000001</v>
       </c>
       <c r="C6" s="1">
-        <v>12.341751695000001</v>
+        <v>11.746712</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1127,7 +1128,7 @@
         <v>10.565674063500001</v>
       </c>
       <c r="C7" s="1">
-        <v>14.565941799999999</v>
+        <v>14.619760100000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1138,7 +1139,7 @@
         <v>22.186550787999998</v>
       </c>
       <c r="C8" s="1">
-        <v>10.404058984000001</v>
+        <v>10.1704145</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1149,7 +1150,7 @@
         <v>27.562345714999999</v>
       </c>
       <c r="C9" s="1">
-        <v>23.378130599999999</v>
+        <v>23.058410299999998</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1160,7 +1161,7 @@
         <v>21.088647905779997</v>
       </c>
       <c r="C10" s="1">
-        <v>14.196419000000001</v>
+        <v>14.072506799999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1171,7 +1172,7 @@
         <v>18.630064737999998</v>
       </c>
       <c r="C11" s="1">
-        <v>13.919755455799999</v>
+        <v>38.941495600000003</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1182,7 +1183,7 @@
         <v>20.465125691120001</v>
       </c>
       <c r="C12" s="1">
-        <v>23.662476788000003</v>
+        <v>67.316375899999997</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1193,7 +1194,7 @@
         <v>14.031910436199999</v>
       </c>
       <c r="C13" s="1">
-        <v>13.130050776999999</v>
+        <v>21.3923387</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1204,7 +1205,7 @@
         <v>17.351059494974404</v>
       </c>
       <c r="C14" s="1">
-        <v>9.3312188690000006</v>
+        <v>2.3051662999999998</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1460,7 +1461,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1530,7 +1531,7 @@
         <v>27.27</v>
       </c>
       <c r="E4" s="1">
-        <v>30.227573322000005</v>
+        <v>27.614460697000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1547,7 +1548,7 @@
         <v>27.27</v>
       </c>
       <c r="E5" s="1">
-        <v>32.60451681</v>
+        <v>29.597379536999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1564,7 +1565,7 @@
         <v>27.27</v>
       </c>
       <c r="E6" s="1">
-        <v>28.724957527000011</v>
+        <v>24.333428848000011</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1581,7 +1582,7 @@
         <v>27.27</v>
       </c>
       <c r="E7" s="1">
-        <v>25.169769212999988</v>
+        <v>22.434157786999993</v>
       </c>
     </row>
   </sheetData>
@@ -1599,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Improved ui for chatbot
</commit_message>
<xml_diff>
--- a/dashboard/KAM_Dashboard_FY26.xlsx
+++ b/dashboard/KAM_Dashboard_FY26.xlsx
@@ -542,7 +542,7 @@
         <v>Capability Development in AI</v>
       </c>
       <c r="C2" t="str">
-        <v>amber</v>
+        <v>red</v>
       </c>
     </row>
     <row r="3">
@@ -553,7 +553,7 @@
         <v>Published Account Strategy</v>
       </c>
       <c r="C3" t="str">
-        <v>amber</v>
+        <v>red</v>
       </c>
     </row>
     <row r="4">
@@ -564,7 +564,7 @@
         <v>Architecture &amp; Domain Knowledge</v>
       </c>
       <c r="C4" t="str">
-        <v>amber</v>
+        <v>red</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change NPS achievement to improvement-based calculation
NPS achievement is now calculated as:
  (Year-end NPS - Q1 Baseline) / (Target NPS - Q1 Baseline)

KAM: Baseline=-33, Current=-12, Target=+19 → 21/52 = 40.4%
SALES: Baseline=-30, Current=-12, Target=+19 → 18/49 = 36.7%

- Added Baseline (Q1) column to Excel Annual KPIs sheet
- Parser reads baseline for NPS metric
- NPS tile shows improvement journey (baseline → current → target)
- Drill-down explains the full calculation with formula breakdown
- Takeaways updated to reflect improvement progress

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dashboard/KAM_Dashboard_FY26.xlsx
+++ b/dashboard/KAM_Dashboard_FY26.xlsx
@@ -41,9 +41,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -407,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -444,6 +443,9 @@
       <c r="C3" t="str">
         <v>Achievement Till Date</v>
       </c>
+      <c r="D3" t="str">
+        <v>Baseline (Q1)</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -472,10 +474,13 @@
         <v>NPS Score</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>-11</v>
+        <v>-12</v>
+      </c>
+      <c r="D6">
+        <v>-33</v>
       </c>
     </row>
     <row r="7">
@@ -501,12 +506,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -517,11 +518,6 @@
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -568,6 +564,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
@@ -576,7 +573,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -749,7 +746,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -936,7 +933,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1024,7 +1021,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1645,6 +1642,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C16"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Pushed the bubble up
</commit_message>
<xml_diff>
--- a/dashboard/KAM_Dashboard_FY26.xlsx
+++ b/dashboard/KAM_Dashboard_FY26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://crmnext-my.sharepoint.com/personal/devansh_goel_businessnext_com/Documents/Desktop/New folder/Code/dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_3C045957ADE34C9561875593809EA984A19A1B19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C51FBB8D-160B-44D1-8997-EA43154D62AE}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_3C045957ADE34C9561875593809EA984A19A1B19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B9BF10D-3301-4BB5-A373-2E14FDAE8550}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual KPIs" sheetId="1" r:id="rId1"/>
@@ -759,11 +759,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.58203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -871,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>